<commit_message>
Add license test to Excel design doc
</commit_message>
<xml_diff>
--- a/Design Docs/Grading System.xlsx
+++ b/Design Docs/Grading System.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iosef\OneDrive\Documents\GitHub\arithmetic-tester\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iosef\OneDrive\Documents\GitHub\arithmetic-tester\Design Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Impossible</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Total Number of Guesses</t>
+  </si>
+  <si>
+    <t>Copyright (c) 2017 Matthew Wright.
+Licensed under MIT License. See LICENSE.txt for further details.
+This software should be distributed with a LICENSE.TXT file in the solution root.
+Alternatively  you can find a copy of the license in the github repository:
+https://github.com/wiganlatics/temperature-converter.
+The MIT License text is also available at: https://choosealicense.com/licenses/mit/.
+d</t>
   </si>
 </sst>
 </file>
@@ -104,16 +113,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -319,17 +329,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -357,11 +415,44 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -698,1162 +789,1218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="15" max="15" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="29" t="s">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="16"/>
-      <c r="C2" s="17">
-        <v>0</v>
-      </c>
-      <c r="D2" s="17">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+    </row>
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15">
+        <v>0</v>
+      </c>
+      <c r="D2" s="15">
         <v>1</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="15">
         <v>2</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="15">
         <v>3</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="15">
         <v>4</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="15">
         <v>5</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="15">
         <v>6</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="15">
         <v>7</v>
       </c>
-      <c r="K2" s="17">
+      <c r="K2" s="15">
         <v>8</v>
       </c>
-      <c r="L2" s="17">
+      <c r="L2" s="15">
         <v>9</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="16">
         <v>10</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="12">
         <v>10</v>
       </c>
-      <c r="C3" s="4">
-        <f>C$2/$B3</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <f>D$2/$B3</f>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:M12" si="0">C$2/$B3</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="E3" s="4">
-        <f>E$2/$B3</f>
+      <c r="E3" s="2">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F3" s="4">
-        <f>F$2/$B3</f>
+      <c r="F3" s="2">
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="G3" s="4">
-        <f>G$2/$B3</f>
+      <c r="G3" s="2">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="H3" s="4">
-        <f>H$2/$B3</f>
+      <c r="H3" s="2">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="I3" s="4">
-        <f>I$2/$B3</f>
+      <c r="I3" s="2">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="J3" s="4">
-        <f>J$2/$B3</f>
+      <c r="J3" s="2">
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="K3" s="4">
-        <f>K$2/$B3</f>
+      <c r="K3" s="2">
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="L3" s="4">
-        <f>L$2/$B3</f>
+      <c r="L3" s="2">
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="M3" s="5">
-        <f>M$2/$B3</f>
+      <c r="M3" s="3">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="O3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="20">
+      <c r="P3" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="14">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="12">
         <v>11</v>
       </c>
-      <c r="C4" s="4">
-        <f>C$2/$B4</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <f>D$2/$B4</f>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="E4" s="4">
-        <f>E$2/$B4</f>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="F4" s="4">
-        <f>F$2/$B4</f>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
         <v>0.27272727272727271</v>
       </c>
-      <c r="G4" s="4">
-        <f>G$2/$B4</f>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
         <v>0.36363636363636365</v>
       </c>
-      <c r="H4" s="4">
-        <f>H$2/$B4</f>
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="I4" s="4">
-        <f>I$2/$B4</f>
+      <c r="I4" s="2">
+        <f t="shared" si="0"/>
         <v>0.54545454545454541</v>
       </c>
-      <c r="J4" s="4">
-        <f>J$2/$B4</f>
+      <c r="J4" s="2">
+        <f t="shared" si="0"/>
         <v>0.63636363636363635</v>
       </c>
-      <c r="K4" s="4">
-        <f>K$2/$B4</f>
+      <c r="K4" s="2">
+        <f t="shared" si="0"/>
         <v>0.72727272727272729</v>
       </c>
-      <c r="L4" s="6">
-        <f>L$2/$B4</f>
+      <c r="L4" s="4">
+        <f t="shared" si="0"/>
         <v>0.81818181818181823</v>
       </c>
-      <c r="M4" s="7">
-        <f>M$2/$B4</f>
+      <c r="M4" s="5">
+        <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="22" t="s">
+      <c r="P4" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="14">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="12">
         <v>12</v>
       </c>
-      <c r="C5" s="4">
-        <f>C$2/$B5</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <f>D$2/$B5</f>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E5" s="4">
-        <f>E$2/$B5</f>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="F5" s="4">
-        <f>F$2/$B5</f>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="G5" s="4">
-        <f>G$2/$B5</f>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="H5" s="4">
-        <f>H$2/$B5</f>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="I5" s="4">
-        <f>I$2/$B5</f>
+      <c r="I5" s="2">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J5" s="4">
-        <f>J$2/$B5</f>
+      <c r="J5" s="2">
+        <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="K5" s="6">
-        <f>K$2/$B5</f>
+      <c r="K5" s="4">
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="L5" s="6">
-        <f>L$2/$B5</f>
+      <c r="L5" s="4">
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="M5" s="7">
-        <f>M$2/$B5</f>
+      <c r="M5" s="5">
+        <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="14">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="12">
         <v>13</v>
       </c>
-      <c r="C6" s="4">
-        <f>C$2/$B6</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <f>D$2/$B6</f>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="E6" s="4">
-        <f>E$2/$B6</f>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
         <v>0.15384615384615385</v>
       </c>
-      <c r="F6" s="4">
-        <f>F$2/$B6</f>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
         <v>0.23076923076923078</v>
       </c>
-      <c r="G6" s="4">
-        <f>G$2/$B6</f>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
         <v>0.30769230769230771</v>
       </c>
-      <c r="H6" s="4">
-        <f>H$2/$B6</f>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
         <v>0.38461538461538464</v>
       </c>
-      <c r="I6" s="4">
-        <f>I$2/$B6</f>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
         <v>0.46153846153846156</v>
       </c>
-      <c r="J6" s="8">
-        <f>J$2/$B6</f>
+      <c r="J6" s="6">
+        <f t="shared" si="0"/>
         <v>0.53846153846153844</v>
       </c>
-      <c r="K6" s="6">
-        <f>K$2/$B6</f>
+      <c r="K6" s="4">
+        <f t="shared" si="0"/>
         <v>0.61538461538461542</v>
       </c>
-      <c r="L6" s="4">
-        <f>L$2/$B6</f>
+      <c r="L6" s="2">
+        <f t="shared" si="0"/>
         <v>0.69230769230769229</v>
       </c>
-      <c r="M6" s="7">
-        <f>M$2/$B6</f>
+      <c r="M6" s="5">
+        <f t="shared" si="0"/>
         <v>0.76923076923076927</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="P6" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="14">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="27"/>
+      <c r="B7" s="12">
         <v>14</v>
       </c>
-      <c r="C7" s="4">
-        <f>C$2/$B7</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <f>D$2/$B7</f>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="E7" s="4">
-        <f>E$2/$B7</f>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="F7" s="4">
-        <f>F$2/$B7</f>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
         <v>0.21428571428571427</v>
       </c>
-      <c r="G7" s="4">
-        <f>G$2/$B7</f>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="H7" s="4">
-        <f>H$2/$B7</f>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
         <v>0.35714285714285715</v>
       </c>
-      <c r="I7" s="8">
-        <f>I$2/$B7</f>
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="J7" s="8">
-        <f>J$2/$B7</f>
+      <c r="J7" s="6">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="K7" s="6">
-        <f>K$2/$B7</f>
+      <c r="K7" s="4">
+        <f t="shared" si="0"/>
         <v>0.5714285714285714</v>
       </c>
-      <c r="L7" s="4">
-        <f>L$2/$B7</f>
+      <c r="L7" s="2">
+        <f t="shared" si="0"/>
         <v>0.6428571428571429</v>
       </c>
-      <c r="M7" s="7">
-        <f>M$2/$B7</f>
+      <c r="M7" s="5">
+        <f t="shared" si="0"/>
         <v>0.7142857142857143</v>
       </c>
-      <c r="O7" s="25" t="s">
+      <c r="O7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="26" t="s">
+      <c r="P7" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="14">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="12">
         <v>15</v>
       </c>
-      <c r="C8" s="4">
-        <f>C$2/$B8</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <f>D$2/$B8</f>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="E8" s="4">
-        <f>E$2/$B8</f>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="F8" s="4">
-        <f>F$2/$B8</f>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="G8" s="4">
-        <f>G$2/$B8</f>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
         <v>0.26666666666666666</v>
       </c>
-      <c r="H8" s="8">
-        <f>H$2/$B8</f>
+      <c r="H8" s="6">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I8" s="8">
-        <f>I$2/$B8</f>
+      <c r="I8" s="6">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="J8" s="8">
-        <f>J$2/$B8</f>
+      <c r="J8" s="6">
+        <f t="shared" si="0"/>
         <v>0.46666666666666667</v>
       </c>
-      <c r="K8" s="4">
-        <f>K$2/$B8</f>
+      <c r="K8" s="2">
+        <f t="shared" si="0"/>
         <v>0.53333333333333333</v>
       </c>
-      <c r="L8" s="4">
-        <f>L$2/$B8</f>
+      <c r="L8" s="2">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="M8" s="7">
-        <f>M$2/$B8</f>
+      <c r="M8" s="5">
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="O8" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="P8" s="28"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="14">
+      <c r="O8" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" s="26"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="12">
         <v>16</v>
       </c>
-      <c r="C9" s="4">
-        <f>C$2/$B9</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <f>D$2/$B9</f>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="E9" s="4">
-        <f>E$2/$B9</f>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="F9" s="4">
-        <f>F$2/$B9</f>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
-      <c r="G9" s="9">
-        <f>G$2/$B9</f>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="H9" s="8">
-        <f>H$2/$B9</f>
+      <c r="H9" s="6">
+        <f t="shared" si="0"/>
         <v>0.3125</v>
       </c>
-      <c r="I9" s="8">
-        <f>I$2/$B9</f>
+      <c r="I9" s="6">
+        <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
-      <c r="J9" s="8">
-        <f>J$2/$B9</f>
+      <c r="J9" s="6">
+        <f t="shared" si="0"/>
         <v>0.4375</v>
       </c>
-      <c r="K9" s="4">
-        <f>K$2/$B9</f>
+      <c r="K9" s="2">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="L9" s="4">
-        <f>L$2/$B9</f>
+      <c r="L9" s="2">
+        <f t="shared" si="0"/>
         <v>0.5625</v>
       </c>
-      <c r="M9" s="7">
-        <f>M$2/$B9</f>
+      <c r="M9" s="5">
+        <f t="shared" si="0"/>
         <v>0.625</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="14">
+    <row r="10" spans="1:20" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
+      <c r="B10" s="12">
         <v>17</v>
       </c>
-      <c r="C10" s="4">
-        <f>C$2/$B10</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <f>D$2/$B10</f>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="E10" s="4">
-        <f>E$2/$B10</f>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
         <v>0.11764705882352941</v>
       </c>
-      <c r="F10" s="9">
-        <f>F$2/$B10</f>
+      <c r="F10" s="7">
+        <f t="shared" si="0"/>
         <v>0.17647058823529413</v>
       </c>
-      <c r="G10" s="9">
-        <f>G$2/$B10</f>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
         <v>0.23529411764705882</v>
       </c>
-      <c r="H10" s="9">
-        <f>H$2/$B10</f>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
         <v>0.29411764705882354</v>
       </c>
-      <c r="I10" s="8">
-        <f>I$2/$B10</f>
+      <c r="I10" s="6">
+        <f t="shared" si="0"/>
         <v>0.35294117647058826</v>
       </c>
-      <c r="J10" s="4">
-        <f>J$2/$B10</f>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
         <v>0.41176470588235292</v>
       </c>
-      <c r="K10" s="4">
-        <f>K$2/$B10</f>
+      <c r="K10" s="2">
+        <f t="shared" si="0"/>
         <v>0.47058823529411764</v>
       </c>
-      <c r="L10" s="4">
-        <f>L$2/$B10</f>
+      <c r="L10" s="2">
+        <f t="shared" si="0"/>
         <v>0.52941176470588236</v>
       </c>
-      <c r="M10" s="7">
-        <f>M$2/$B10</f>
+      <c r="M10" s="5">
+        <f t="shared" si="0"/>
         <v>0.58823529411764708</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="14">
+    <row r="11" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
+      <c r="B11" s="12">
         <v>18</v>
       </c>
-      <c r="C11" s="4">
-        <f>C$2/$B11</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <f>D$2/$B11</f>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="E11" s="9">
-        <f>E$2/$B11</f>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="F11" s="9">
-        <f>F$2/$B11</f>
+      <c r="F11" s="7">
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G11" s="9">
-        <f>G$2/$B11</f>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
         <v>0.22222222222222221</v>
       </c>
-      <c r="H11" s="9">
-        <f>H$2/$B11</f>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
         <v>0.27777777777777779</v>
       </c>
-      <c r="I11" s="8">
-        <f>I$2/$B11</f>
+      <c r="I11" s="6">
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J11" s="4">
-        <f>J$2/$B11</f>
+      <c r="J11" s="2">
+        <f t="shared" si="0"/>
         <v>0.3888888888888889</v>
       </c>
-      <c r="K11" s="4">
-        <f>K$2/$B11</f>
+      <c r="K11" s="2">
+        <f t="shared" si="0"/>
         <v>0.44444444444444442</v>
       </c>
-      <c r="L11" s="4">
-        <f>L$2/$B11</f>
+      <c r="L11" s="2">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="M11" s="7">
-        <f>M$2/$B11</f>
+      <c r="M11" s="5">
+        <f t="shared" si="0"/>
         <v>0.55555555555555558</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="14">
+      <c r="O11" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="31"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="12">
         <v>19</v>
       </c>
-      <c r="C12" s="4">
-        <f>C$2/$B12</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="10">
-        <f>D$2/$B12</f>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
         <v>5.2631578947368418E-2</v>
       </c>
-      <c r="E12" s="9">
-        <f>E$2/$B12</f>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
         <v>0.10526315789473684</v>
       </c>
-      <c r="F12" s="9">
-        <f>F$2/$B12</f>
+      <c r="F12" s="7">
+        <f t="shared" si="0"/>
         <v>0.15789473684210525</v>
       </c>
-      <c r="G12" s="9">
-        <f>G$2/$B12</f>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
         <v>0.21052631578947367</v>
       </c>
-      <c r="H12" s="9">
-        <f>H$2/$B12</f>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
         <v>0.26315789473684209</v>
       </c>
-      <c r="I12" s="4">
-        <f>I$2/$B12</f>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
         <v>0.31578947368421051</v>
       </c>
-      <c r="J12" s="4">
-        <f>J$2/$B12</f>
+      <c r="J12" s="2">
+        <f t="shared" si="0"/>
         <v>0.36842105263157893</v>
       </c>
-      <c r="K12" s="4">
-        <f>K$2/$B12</f>
+      <c r="K12" s="2">
+        <f t="shared" si="0"/>
         <v>0.42105263157894735</v>
       </c>
-      <c r="L12" s="4">
-        <f>L$2/$B12</f>
+      <c r="L12" s="2">
+        <f t="shared" si="0"/>
         <v>0.47368421052631576</v>
       </c>
-      <c r="M12" s="7">
-        <f>M$2/$B12</f>
+      <c r="M12" s="5">
+        <f t="shared" si="0"/>
         <v>0.52631578947368418</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="14">
+      <c r="O12" s="32"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="34"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="12">
         <v>20</v>
       </c>
-      <c r="C13" s="10">
-        <f>C$2/$B13</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="10">
-        <f>D$2/$B13</f>
+      <c r="C13" s="8">
+        <f t="shared" ref="C13:M23" si="1">C$2/$B13</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="E13" s="10">
-        <f>E$2/$B13</f>
+      <c r="E13" s="8">
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F13" s="9">
-        <f>F$2/$B13</f>
+      <c r="F13" s="7">
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="G13" s="9">
-        <f>G$2/$B13</f>
+      <c r="G13" s="7">
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="H13" s="9">
-        <f>H$2/$B13</f>
+      <c r="H13" s="7">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="I13" s="4">
-        <f>I$2/$B13</f>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="J13" s="4">
-        <f>J$2/$B13</f>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
         <v>0.35</v>
       </c>
-      <c r="K13" s="4">
-        <f>K$2/$B13</f>
+      <c r="K13" s="2">
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="L13" s="4">
-        <f>L$2/$B13</f>
+      <c r="L13" s="2">
+        <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
-      <c r="M13" s="7">
-        <f>M$2/$B13</f>
+      <c r="M13" s="5">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="14">
+      <c r="O13" s="32"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="34"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="12">
         <v>21</v>
       </c>
-      <c r="C14" s="10">
-        <f>C$2/$B14</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="10">
-        <f>D$2/$B14</f>
+      <c r="C14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="1"/>
         <v>4.7619047619047616E-2</v>
       </c>
-      <c r="E14" s="10">
-        <f>E$2/$B14</f>
+      <c r="E14" s="8">
+        <f t="shared" si="1"/>
         <v>9.5238095238095233E-2</v>
       </c>
-      <c r="F14" s="9">
-        <f>F$2/$B14</f>
+      <c r="F14" s="7">
+        <f t="shared" si="1"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="G14" s="9">
-        <f>G$2/$B14</f>
+      <c r="G14" s="7">
+        <f t="shared" si="1"/>
         <v>0.19047619047619047</v>
       </c>
-      <c r="H14" s="4">
-        <f>H$2/$B14</f>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
         <v>0.23809523809523808</v>
       </c>
-      <c r="I14" s="4">
-        <f>I$2/$B14</f>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="J14" s="4">
-        <f>J$2/$B14</f>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K14" s="4">
-        <f>K$2/$B14</f>
+      <c r="K14" s="2">
+        <f t="shared" si="1"/>
         <v>0.38095238095238093</v>
       </c>
-      <c r="L14" s="4">
-        <f>L$2/$B14</f>
+      <c r="L14" s="2">
+        <f t="shared" si="1"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="M14" s="7">
-        <f>M$2/$B14</f>
+      <c r="M14" s="5">
+        <f t="shared" si="1"/>
         <v>0.47619047619047616</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="14">
+      <c r="O14" s="32"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="34"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="27"/>
+      <c r="B15" s="12">
         <v>22</v>
       </c>
-      <c r="C15" s="10">
-        <f>C$2/$B15</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="10">
-        <f>D$2/$B15</f>
+      <c r="C15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" si="1"/>
         <v>4.5454545454545456E-2</v>
       </c>
-      <c r="E15" s="10">
-        <f>E$2/$B15</f>
+      <c r="E15" s="8">
+        <f t="shared" si="1"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="F15" s="9">
-        <f>F$2/$B15</f>
+      <c r="F15" s="7">
+        <f t="shared" si="1"/>
         <v>0.13636363636363635</v>
       </c>
-      <c r="G15" s="9">
-        <f>G$2/$B15</f>
+      <c r="G15" s="7">
+        <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="H15" s="4">
-        <f>H$2/$B15</f>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
         <v>0.22727272727272727</v>
       </c>
-      <c r="I15" s="4">
-        <f>I$2/$B15</f>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
         <v>0.27272727272727271</v>
       </c>
-      <c r="J15" s="4">
-        <f>J$2/$B15</f>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
         <v>0.31818181818181818</v>
       </c>
-      <c r="K15" s="4">
-        <f>K$2/$B15</f>
+      <c r="K15" s="2">
+        <f t="shared" si="1"/>
         <v>0.36363636363636365</v>
       </c>
-      <c r="L15" s="4">
-        <f>L$2/$B15</f>
+      <c r="L15" s="2">
+        <f t="shared" si="1"/>
         <v>0.40909090909090912</v>
       </c>
-      <c r="M15" s="7">
-        <f>M$2/$B15</f>
+      <c r="M15" s="5">
+        <f t="shared" si="1"/>
         <v>0.45454545454545453</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="14">
+      <c r="O15" s="32"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="34"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="27"/>
+      <c r="B16" s="12">
         <v>23</v>
       </c>
-      <c r="C16" s="10">
-        <f>C$2/$B16</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="10">
-        <f>D$2/$B16</f>
+      <c r="C16" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="8">
+        <f t="shared" si="1"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="E16" s="10">
-        <f>E$2/$B16</f>
+      <c r="E16" s="8">
+        <f t="shared" si="1"/>
         <v>8.6956521739130432E-2</v>
       </c>
-      <c r="F16" s="9">
-        <f>F$2/$B16</f>
+      <c r="F16" s="7">
+        <f t="shared" si="1"/>
         <v>0.13043478260869565</v>
       </c>
-      <c r="G16" s="4">
-        <f>G$2/$B16</f>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
         <v>0.17391304347826086</v>
       </c>
-      <c r="H16" s="4">
-        <f>H$2/$B16</f>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
         <v>0.21739130434782608</v>
       </c>
-      <c r="I16" s="4">
-        <f>I$2/$B16</f>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
         <v>0.2608695652173913</v>
       </c>
-      <c r="J16" s="4">
-        <f>J$2/$B16</f>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
         <v>0.30434782608695654</v>
       </c>
-      <c r="K16" s="4">
-        <f>K$2/$B16</f>
+      <c r="K16" s="2">
+        <f t="shared" si="1"/>
         <v>0.34782608695652173</v>
       </c>
-      <c r="L16" s="4">
-        <f>L$2/$B16</f>
+      <c r="L16" s="2">
+        <f t="shared" si="1"/>
         <v>0.39130434782608697</v>
       </c>
-      <c r="M16" s="7">
-        <f>M$2/$B16</f>
+      <c r="M16" s="5">
+        <f t="shared" si="1"/>
         <v>0.43478260869565216</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="14">
+      <c r="O16" s="32"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="34"/>
+    </row>
+    <row r="17" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="27"/>
+      <c r="B17" s="12">
         <v>24</v>
       </c>
-      <c r="C17" s="10">
-        <f>C$2/$B17</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="10">
-        <f>D$2/$B17</f>
+      <c r="C17" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="8">
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E17" s="10">
-        <f>E$2/$B17</f>
+      <c r="E17" s="8">
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F17" s="9">
-        <f>F$2/$B17</f>
+      <c r="F17" s="7">
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="G17" s="4">
-        <f>G$2/$B17</f>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="H17" s="4">
-        <f>H$2/$B17</f>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
         <v>0.20833333333333334</v>
       </c>
-      <c r="I17" s="4">
-        <f>I$2/$B17</f>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="J17" s="4">
-        <f>J$2/$B17</f>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
         <v>0.29166666666666669</v>
       </c>
-      <c r="K17" s="4">
-        <f>K$2/$B17</f>
+      <c r="K17" s="2">
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="L17" s="4">
-        <f>L$2/$B17</f>
+      <c r="L17" s="2">
+        <f t="shared" si="1"/>
         <v>0.375</v>
       </c>
-      <c r="M17" s="7">
-        <f>M$2/$B17</f>
+      <c r="M17" s="5">
+        <f t="shared" si="1"/>
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="14">
+      <c r="O17" s="35"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="37"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="27"/>
+      <c r="B18" s="12">
         <v>25</v>
       </c>
-      <c r="C18" s="10">
-        <f>C$2/$B18</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="10">
-        <f>D$2/$B18</f>
+      <c r="C18" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="8">
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
-      <c r="E18" s="10">
-        <f>E$2/$B18</f>
+      <c r="E18" s="8">
+        <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
-      <c r="F18" s="4">
-        <f>F$2/$B18</f>
+      <c r="F18" s="2">
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
-      <c r="G18" s="4">
-        <f>G$2/$B18</f>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="H18" s="4">
-        <f>H$2/$B18</f>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="I18" s="4">
-        <f>I$2/$B18</f>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="J18" s="4">
-        <f>J$2/$B18</f>
+      <c r="J18" s="2">
+        <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="K18" s="4">
-        <f>K$2/$B18</f>
+      <c r="K18" s="2">
+        <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
-      <c r="L18" s="4">
-        <f>L$2/$B18</f>
+      <c r="L18" s="2">
+        <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="M18" s="7">
-        <f>M$2/$B18</f>
+      <c r="M18" s="5">
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="14">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="27"/>
+      <c r="B19" s="12">
         <v>26</v>
       </c>
-      <c r="C19" s="10">
-        <f>C$2/$B19</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="10">
-        <f>D$2/$B19</f>
+      <c r="C19" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="8">
+        <f t="shared" si="1"/>
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="E19" s="10">
-        <f>E$2/$B19</f>
+      <c r="E19" s="8">
+        <f t="shared" si="1"/>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="F19" s="4">
-        <f>F$2/$B19</f>
+      <c r="F19" s="2">
+        <f t="shared" si="1"/>
         <v>0.11538461538461539</v>
       </c>
-      <c r="G19" s="4">
-        <f>G$2/$B19</f>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
         <v>0.15384615384615385</v>
       </c>
-      <c r="H19" s="4">
-        <f>H$2/$B19</f>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
         <v>0.19230769230769232</v>
       </c>
-      <c r="I19" s="4">
-        <f>I$2/$B19</f>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
         <v>0.23076923076923078</v>
       </c>
-      <c r="J19" s="4">
-        <f>J$2/$B19</f>
+      <c r="J19" s="2">
+        <f t="shared" si="1"/>
         <v>0.26923076923076922</v>
       </c>
-      <c r="K19" s="4">
-        <f>K$2/$B19</f>
+      <c r="K19" s="2">
+        <f t="shared" si="1"/>
         <v>0.30769230769230771</v>
       </c>
-      <c r="L19" s="4">
-        <f>L$2/$B19</f>
+      <c r="L19" s="2">
+        <f t="shared" si="1"/>
         <v>0.34615384615384615</v>
       </c>
-      <c r="M19" s="7">
-        <f>M$2/$B19</f>
+      <c r="M19" s="5">
+        <f t="shared" si="1"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="14">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="27"/>
+      <c r="B20" s="12">
         <v>27</v>
       </c>
-      <c r="C20" s="10">
-        <f>C$2/$B20</f>
-        <v>0</v>
-      </c>
-      <c r="D20" s="10">
-        <f>D$2/$B20</f>
+      <c r="C20" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="8">
+        <f t="shared" si="1"/>
         <v>3.7037037037037035E-2</v>
       </c>
-      <c r="E20" s="4">
-        <f>E$2/$B20</f>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
         <v>7.407407407407407E-2</v>
       </c>
-      <c r="F20" s="4">
-        <f>F$2/$B20</f>
+      <c r="F20" s="2">
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="G20" s="4">
-        <f>G$2/$B20</f>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
         <v>0.14814814814814814</v>
       </c>
-      <c r="H20" s="4">
-        <f>H$2/$B20</f>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
         <v>0.18518518518518517</v>
       </c>
-      <c r="I20" s="4">
-        <f>I$2/$B20</f>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
         <v>0.22222222222222221</v>
       </c>
-      <c r="J20" s="4">
-        <f>J$2/$B20</f>
+      <c r="J20" s="2">
+        <f t="shared" si="1"/>
         <v>0.25925925925925924</v>
       </c>
-      <c r="K20" s="4">
-        <f>K$2/$B20</f>
+      <c r="K20" s="2">
+        <f t="shared" si="1"/>
         <v>0.29629629629629628</v>
       </c>
-      <c r="L20" s="4">
-        <f>L$2/$B20</f>
+      <c r="L20" s="2">
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="M20" s="7">
-        <f>M$2/$B20</f>
+      <c r="M20" s="5">
+        <f t="shared" si="1"/>
         <v>0.37037037037037035</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="14">
+      <c r="O20" s="38"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="27"/>
+      <c r="B21" s="12">
         <v>28</v>
       </c>
-      <c r="C21" s="10">
-        <f>C$2/$B21</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="10">
-        <f>D$2/$B21</f>
+      <c r="C21" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="8">
+        <f t="shared" si="1"/>
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="E21" s="4">
-        <f>E$2/$B21</f>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="F21" s="4">
-        <f>F$2/$B21</f>
+      <c r="F21" s="2">
+        <f t="shared" si="1"/>
         <v>0.10714285714285714</v>
       </c>
-      <c r="G21" s="4">
-        <f>G$2/$B21</f>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="H21" s="4">
-        <f>H$2/$B21</f>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
         <v>0.17857142857142858</v>
       </c>
-      <c r="I21" s="4">
-        <f>I$2/$B21</f>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
         <v>0.21428571428571427</v>
       </c>
-      <c r="J21" s="4">
-        <f>J$2/$B21</f>
+      <c r="J21" s="2">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="K21" s="4">
-        <f>K$2/$B21</f>
+      <c r="K21" s="2">
+        <f t="shared" si="1"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="L21" s="4">
-        <f>L$2/$B21</f>
+      <c r="L21" s="2">
+        <f t="shared" si="1"/>
         <v>0.32142857142857145</v>
       </c>
-      <c r="M21" s="7">
-        <f>M$2/$B21</f>
+      <c r="M21" s="5">
+        <f t="shared" si="1"/>
         <v>0.35714285714285715</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="14">
+      <c r="O21" s="38"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="27"/>
+      <c r="B22" s="12">
         <v>29</v>
       </c>
-      <c r="C22" s="10">
-        <f>C$2/$B22</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="4">
-        <f>D$2/$B22</f>
+      <c r="C22" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="1"/>
         <v>3.4482758620689655E-2</v>
       </c>
-      <c r="E22" s="4">
-        <f>E$2/$B22</f>
+      <c r="E22" s="2">
+        <f t="shared" si="1"/>
         <v>6.8965517241379309E-2</v>
       </c>
-      <c r="F22" s="4">
-        <f>F$2/$B22</f>
+      <c r="F22" s="2">
+        <f t="shared" si="1"/>
         <v>0.10344827586206896</v>
       </c>
-      <c r="G22" s="4">
-        <f>G$2/$B22</f>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
         <v>0.13793103448275862</v>
       </c>
-      <c r="H22" s="4">
-        <f>H$2/$B22</f>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
         <v>0.17241379310344829</v>
       </c>
-      <c r="I22" s="4">
-        <f>I$2/$B22</f>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
         <v>0.20689655172413793</v>
       </c>
-      <c r="J22" s="4">
-        <f>J$2/$B22</f>
+      <c r="J22" s="2">
+        <f t="shared" si="1"/>
         <v>0.2413793103448276</v>
       </c>
-      <c r="K22" s="4">
-        <f>K$2/$B22</f>
+      <c r="K22" s="2">
+        <f t="shared" si="1"/>
         <v>0.27586206896551724</v>
       </c>
-      <c r="L22" s="4">
-        <f>L$2/$B22</f>
+      <c r="L22" s="2">
+        <f t="shared" si="1"/>
         <v>0.31034482758620691</v>
       </c>
-      <c r="M22" s="7">
-        <f>M$2/$B22</f>
+      <c r="M22" s="5">
+        <f t="shared" si="1"/>
         <v>0.34482758620689657</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="15">
+      <c r="O22" s="38"/>
+    </row>
+    <row r="23" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="27"/>
+      <c r="B23" s="13">
         <v>30</v>
       </c>
-      <c r="C23" s="11">
-        <f>C$2/$B23</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="12">
-        <f>D$2/$B23</f>
+      <c r="C23" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" si="1"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="E23" s="12">
-        <f>E$2/$B23</f>
+      <c r="E23" s="10">
+        <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="F23" s="12">
-        <f>F$2/$B23</f>
+      <c r="F23" s="10">
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="G23" s="12">
-        <f>G$2/$B23</f>
+      <c r="G23" s="10">
+        <f t="shared" si="1"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="H23" s="12">
-        <f>H$2/$B23</f>
+      <c r="H23" s="10">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="I23" s="12">
-        <f>I$2/$B23</f>
+      <c r="I23" s="10">
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="J23" s="12">
-        <f>J$2/$B23</f>
+      <c r="J23" s="10">
+        <f t="shared" si="1"/>
         <v>0.23333333333333334</v>
       </c>
-      <c r="K23" s="12">
-        <f>K$2/$B23</f>
+      <c r="K23" s="10">
+        <f t="shared" si="1"/>
         <v>0.26666666666666666</v>
       </c>
-      <c r="L23" s="12">
-        <f>L$2/$B23</f>
+      <c r="L23" s="10">
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="M23" s="13">
-        <f>M$2/$B23</f>
+      <c r="M23" s="11">
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O24" s="2"/>
+      <c r="O23" s="38"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="O24" s="38"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="O25" s="39"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="O26" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="O11:T17"/>
     <mergeCell ref="A3:A23"/>
     <mergeCell ref="C1:M1"/>
   </mergeCells>

</xml_diff>